<commit_message>
alterações para o desafio da 1 unidade
</commit_message>
<xml_diff>
--- a/resultadosJAVASCRIPT_BUBBLE.xlsx
+++ b/resultadosJAVASCRIPT_BUBBLE.xlsx
@@ -418,7 +418,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1670</v>
+        <v>2252</v>
       </c>
       <c r="C2">
         <v>0.265625</v>
@@ -429,7 +429,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1676</v>
+        <v>2559</v>
       </c>
       <c r="C3">
         <v>0.265625</v>
@@ -440,7 +440,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1734</v>
+        <v>2675</v>
       </c>
       <c r="C4">
         <v>0.265625</v>
@@ -451,10 +451,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>1734</v>
+        <v>2731</v>
       </c>
       <c r="C5">
-        <v>0.28125</v>
+        <v>0.265625</v>
       </c>
     </row>
     <row r="6">
@@ -462,7 +462,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1751</v>
+        <v>2782</v>
       </c>
       <c r="C6">
         <v>0.28125</v>
@@ -473,7 +473,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>1763</v>
+        <v>3132</v>
       </c>
       <c r="C7">
         <v>0.28125</v>
@@ -484,7 +484,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>1813</v>
+        <v>3183</v>
       </c>
       <c r="C8">
         <v>0.28125</v>
@@ -495,10 +495,10 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>1909</v>
+        <v>3417</v>
       </c>
       <c r="C9">
-        <v>0.359375</v>
+        <v>0.28125</v>
       </c>
     </row>
     <row r="10">
@@ -506,10 +506,10 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>2026</v>
+        <v>3606</v>
       </c>
       <c r="C10">
-        <v>5.8515625</v>
+        <v>0.359375</v>
       </c>
     </row>
     <row r="11">
@@ -517,10 +517,10 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>2149</v>
+        <v>4093</v>
       </c>
       <c r="C11">
-        <v>249.015625</v>
+        <v>249.109375</v>
       </c>
     </row>
     <row r="13">
@@ -528,10 +528,10 @@
         <v>Média</v>
       </c>
       <c r="B13" t="str">
-        <v>1822.50</v>
+        <v>3043.00</v>
       </c>
       <c r="C13" t="str">
-        <v>25.71</v>
+        <v>25.17</v>
       </c>
     </row>
     <row r="14">
@@ -539,7 +539,7 @@
         <v>Mediana</v>
       </c>
       <c r="B14" t="str">
-        <v>1757.00</v>
+        <v>2957.00</v>
       </c>
       <c r="C14" t="str">
         <v>0.28</v>

</xml_diff>